<commit_message>
Edit raw data file
</commit_message>
<xml_diff>
--- a/models/Council-Backlog-Raw.xlsx
+++ b/models/Council-Backlog-Raw.xlsx
@@ -2,23 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
-  <workbookPr showInkAnnotation="0"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawoleoni/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawoleoni/Documents/workspace/BARP-New/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E464D14E-3A3E-BF4D-9ADD-4ED46B6111E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B517F29-2A31-F44E-AA16-A8143795A323}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="740" windowWidth="21500" windowHeight="15460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3640" yWindow="1880" windowWidth="21500" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning Parameters" sheetId="5" r:id="rId1"/>
     <sheet name="Backlog &amp; dependencies" sheetId="2" r:id="rId2"/>
-    <sheet name="Effort Estimates" sheetId="3" r:id="rId3"/>
-    <sheet name="Effort Estimates (EL)" sheetId="7" r:id="rId4"/>
-    <sheet name="Value Estimates (EL)" sheetId="8" r:id="rId5"/>
-    <sheet name="BEARS input" sheetId="1" r:id="rId6"/>
+    <sheet name="Effort Estimates" sheetId="7" r:id="rId3"/>
+    <sheet name="Value Estimates" sheetId="8" r:id="rId4"/>
+    <sheet name="BEARS input" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="80">
   <si>
     <t>Work Item</t>
   </si>
@@ -199,9 +198,6 @@
     <t>5. Interface to Council Housing Repository</t>
   </si>
   <si>
-    <t>All estimates are in man-hours</t>
-  </si>
-  <si>
     <t>F. apply for parking permit</t>
   </si>
   <si>
@@ -275,6 +271,9 @@
   </si>
   <si>
     <t>6. Interface to parking fine system</t>
+  </si>
+  <si>
+    <t>3,6</t>
   </si>
 </sst>
 </file>
@@ -646,10 +645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,7 +671,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -708,11 +708,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,7 +795,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="str">
         <f>B2</f>
@@ -811,7 +812,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="str">
         <f>A21</f>
@@ -828,19 +829,19 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
       <c r="C9" t="str">
-        <f>A9</f>
-        <v>H. Pay parking and traffic fine</v>
+        <f>A26</f>
+        <v>6. Interface to parking fine system</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="str">
         <f>A24</f>
@@ -849,7 +850,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="str">
         <f>A22</f>
@@ -862,7 +863,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="str">
         <f>A21</f>
@@ -875,7 +876,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" t="str">
         <f>A25</f>
@@ -884,7 +885,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="str">
         <f>A25</f>
@@ -893,7 +894,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" t="str">
         <f>A23</f>
@@ -902,7 +903,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" t="str">
         <f>A21</f>
@@ -911,7 +912,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" t="str">
         <f>A15</f>
@@ -920,12 +921,12 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="str">
         <f>A26</f>
@@ -934,7 +935,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -964,7 +965,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -973,12 +974,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1024,25 +1026,25 @@
         <v>30</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
         <v>30</v>
       </c>
-      <c r="C2">
-        <v>45</v>
-      </c>
-      <c r="D2">
-        <v>55</v>
-      </c>
-      <c r="E2">
-        <v>60</v>
-      </c>
-      <c r="F2">
-        <v>70</v>
-      </c>
       <c r="G2">
-        <v>3.9710000000000001</v>
+        <v>1.7470000000000001</v>
       </c>
       <c r="H2">
-        <v>0.193</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1050,25 +1052,25 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>95</v>
+        <v>15</v>
       </c>
       <c r="E3">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="F3">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G3">
-        <v>4.5659999999999998</v>
+        <v>2.61</v>
       </c>
       <c r="H3">
-        <v>0.14299999999999999</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1076,25 +1078,25 @@
         <v>32</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
         <v>20</v>
       </c>
-      <c r="C4">
-        <v>25</v>
-      </c>
-      <c r="D4">
-        <v>33</v>
-      </c>
-      <c r="E4">
-        <v>45</v>
-      </c>
-      <c r="F4">
-        <v>50</v>
-      </c>
       <c r="G4">
-        <v>3.492</v>
+        <v>1.88</v>
       </c>
       <c r="H4">
-        <v>0.32200000000000001</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1102,25 +1104,27 @@
         <v>33</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
         <v>30</v>
       </c>
-      <c r="F5">
-        <v>35</v>
-      </c>
       <c r="G5">
-        <v>3.1760000000000002</v>
+        <f>G2</f>
+        <v>1.7470000000000001</v>
       </c>
       <c r="H5">
-        <v>0.29199999999999998</v>
+        <f>H2</f>
+        <v>0.73</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1128,415 +1132,429 @@
         <v>34</v>
       </c>
       <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6">
         <v>30</v>
       </c>
-      <c r="C6">
-        <v>45</v>
-      </c>
-      <c r="D6">
-        <v>55</v>
-      </c>
-      <c r="E6">
-        <v>75</v>
-      </c>
-      <c r="F6">
-        <v>90</v>
-      </c>
       <c r="G6">
-        <v>4.0259999999999998</v>
+        <v>2.35</v>
       </c>
       <c r="H6">
-        <v>0.32200000000000001</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="F7">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="G7">
-        <v>4.4530000000000003</v>
+        <f>G3</f>
+        <v>2.61</v>
       </c>
       <c r="H7">
-        <v>0.23699999999999999</v>
+        <f>H3</f>
+        <v>0.65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
         <v>30</v>
       </c>
-      <c r="D8">
-        <v>35</v>
-      </c>
-      <c r="E8">
-        <v>45</v>
-      </c>
-      <c r="F8">
-        <v>50</v>
-      </c>
       <c r="G8">
-        <v>3.5680000000000001</v>
+        <v>2.21</v>
       </c>
       <c r="H8">
-        <v>0.251</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>22</v>
+      </c>
+      <c r="F9">
         <v>30</v>
       </c>
-      <c r="C9">
-        <v>35</v>
-      </c>
-      <c r="D9">
-        <v>45</v>
-      </c>
-      <c r="E9">
-        <v>60</v>
-      </c>
-      <c r="F9">
-        <v>75</v>
-      </c>
       <c r="G9">
-        <v>3.823</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="H9">
-        <v>0.309</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
         <v>20</v>
       </c>
-      <c r="C10">
-        <v>25</v>
-      </c>
-      <c r="D10">
-        <v>28</v>
-      </c>
-      <c r="E10">
-        <v>32</v>
-      </c>
-      <c r="F10">
-        <v>35</v>
-      </c>
       <c r="G10">
-        <v>3.3319999999999999</v>
+        <v>1.98</v>
       </c>
       <c r="H10">
-        <v>0.156</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F11">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="G11">
-        <v>3.3319999999999999</v>
+        <f>G10</f>
+        <v>1.98</v>
       </c>
       <c r="H11">
-        <v>0.157</v>
+        <f>H10</f>
+        <v>0.71</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E12">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="F12">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G12">
-        <v>3.5510000000000002</v>
+        <f>G10</f>
+        <v>1.98</v>
       </c>
       <c r="H12">
-        <v>0.192</v>
+        <f>H10</f>
+        <v>0.71</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
         <v>40</v>
       </c>
-      <c r="C13">
-        <v>60</v>
-      </c>
-      <c r="D13">
-        <v>70</v>
-      </c>
-      <c r="E13">
-        <v>80</v>
-      </c>
-      <c r="F13">
-        <v>100</v>
-      </c>
       <c r="G13">
-        <v>4.2409999999999997</v>
+        <f>G3</f>
+        <v>2.61</v>
       </c>
       <c r="H13">
-        <v>0.20200000000000001</v>
+        <f>H3</f>
+        <v>0.65</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="E14">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="F14">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="G14">
-        <v>3.827</v>
+        <f>G10</f>
+        <v>1.98</v>
       </c>
       <c r="H14">
-        <v>0.317</v>
+        <f>H10</f>
+        <v>0.71</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="D15">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="E15">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="F15">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="G15">
-        <v>4.306</v>
+        <v>2.98</v>
       </c>
       <c r="H15">
-        <v>0.191</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="E16">
+        <v>12</v>
+      </c>
+      <c r="F16">
         <v>20</v>
       </c>
-      <c r="C16">
-        <v>30</v>
-      </c>
-      <c r="D16">
-        <v>35</v>
-      </c>
-      <c r="E16">
-        <v>45</v>
-      </c>
-      <c r="F16">
-        <v>50</v>
-      </c>
       <c r="G16">
-        <v>3.5680000000000001</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="H16">
-        <v>0.251</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="F17">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>3.4980000000000002</v>
+        <v>1.37</v>
       </c>
       <c r="H17">
-        <v>0.29399999999999998</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="E18">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="F18">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>3.5219999999999998</v>
+        <f>G17</f>
+        <v>1.37</v>
       </c>
       <c r="H18">
-        <v>0.13300000000000001</v>
+        <f>H17</f>
+        <v>0.38</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E19">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="F19">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="G19">
-        <v>4.0190000000000001</v>
+        <f>G8</f>
+        <v>2.21</v>
       </c>
       <c r="H19">
-        <v>0.16300000000000001</v>
+        <f>H8</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E20">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F20">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>3.306</v>
+        <v>1.3</v>
       </c>
       <c r="H20">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
       <c r="B21">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="D21">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="E21">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="F21">
-        <v>60</v>
-      </c>
-      <c r="G21">
-        <v>3.819</v>
-      </c>
-      <c r="H21">
-        <v>0.19800000000000001</v>
+        <v>20</v>
+      </c>
+      <c r="G21" s="9">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0.59</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1544,25 +1562,25 @@
         <v>36</v>
       </c>
       <c r="B22">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>18</v>
+      </c>
+      <c r="F22">
         <v>30</v>
       </c>
-      <c r="D22">
-        <v>35</v>
-      </c>
-      <c r="E22">
-        <v>40</v>
-      </c>
-      <c r="F22">
-        <v>50</v>
-      </c>
       <c r="G22">
-        <v>3.5510000000000002</v>
+        <v>2.61</v>
       </c>
       <c r="H22">
-        <v>0.192</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1570,25 +1588,25 @@
         <v>37</v>
       </c>
       <c r="B23">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="D23">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="E23">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="F23">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="G23">
-        <v>4.2839999999999998</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="H23">
-        <v>0.25800000000000001</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1596,25 +1614,27 @@
         <v>52</v>
       </c>
       <c r="B24">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C24">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D24">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E24">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F24">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G24">
-        <v>3.415</v>
+        <f>G22</f>
+        <v>2.61</v>
       </c>
       <c r="H24">
-        <v>0.21299999999999999</v>
+        <f>H22</f>
+        <v>0.42</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1622,30 +1642,67 @@
         <v>53</v>
       </c>
       <c r="B25">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="E25">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="F25">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G25">
-        <v>3.8530000000000002</v>
+        <f>G22</f>
+        <v>2.61</v>
       </c>
       <c r="H25">
-        <v>0.16400000000000001</v>
+        <f>H22</f>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="str">
+        <f>'Backlog &amp; dependencies'!A26</f>
+        <v>6. Interface to parking fine system</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>14</v>
+      </c>
+      <c r="E26">
+        <v>18</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
+      </c>
+      <c r="G26">
+        <f>G22</f>
+        <v>2.61</v>
+      </c>
+      <c r="H26">
+        <f>H22</f>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <f>SUM(D2:D26)</f>
+        <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="G28" t="s">
         <v>46</v>
@@ -1658,751 +1715,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:H26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="43.5" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>'Backlog &amp; dependencies'!A1</f>
-        <v>Work Items</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>30</v>
-      </c>
-      <c r="G2">
-        <v>1.7470000000000001</v>
-      </c>
-      <c r="H2">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>20</v>
-      </c>
-      <c r="F3">
-        <v>40</v>
-      </c>
-      <c r="G3">
-        <v>2.61</v>
-      </c>
-      <c r="H3">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <v>1.88</v>
-      </c>
-      <c r="H4">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>30</v>
-      </c>
-      <c r="G5">
-        <f>G2</f>
-        <v>1.7470000000000001</v>
-      </c>
-      <c r="H5">
-        <f>H2</f>
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>18</v>
-      </c>
-      <c r="F6">
-        <v>30</v>
-      </c>
-      <c r="G6">
-        <v>2.35</v>
-      </c>
-      <c r="H6">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>15</v>
-      </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <v>40</v>
-      </c>
-      <c r="G7">
-        <f>G3</f>
-        <v>2.61</v>
-      </c>
-      <c r="H7">
-        <f>H3</f>
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>15</v>
-      </c>
-      <c r="F8">
-        <v>30</v>
-      </c>
-      <c r="G8">
-        <v>2.21</v>
-      </c>
-      <c r="H8">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <v>22</v>
-      </c>
-      <c r="F9">
-        <v>30</v>
-      </c>
-      <c r="G9">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="H9">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10">
-        <v>12</v>
-      </c>
-      <c r="F10">
-        <v>20</v>
-      </c>
-      <c r="G10">
-        <v>1.98</v>
-      </c>
-      <c r="H10">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>12</v>
-      </c>
-      <c r="F11">
-        <v>20</v>
-      </c>
-      <c r="G11">
-        <f>G10</f>
-        <v>1.98</v>
-      </c>
-      <c r="H11">
-        <f>H10</f>
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>8</v>
-      </c>
-      <c r="E12">
-        <v>12</v>
-      </c>
-      <c r="F12">
-        <v>20</v>
-      </c>
-      <c r="G12">
-        <f>G10</f>
-        <v>1.98</v>
-      </c>
-      <c r="H12">
-        <f>H10</f>
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>8</v>
-      </c>
-      <c r="D13">
-        <v>15</v>
-      </c>
-      <c r="E13">
-        <v>20</v>
-      </c>
-      <c r="F13">
-        <v>40</v>
-      </c>
-      <c r="G13">
-        <f>G3</f>
-        <v>2.61</v>
-      </c>
-      <c r="H13">
-        <f>H3</f>
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <v>12</v>
-      </c>
-      <c r="F14">
-        <v>20</v>
-      </c>
-      <c r="G14">
-        <f>G10</f>
-        <v>1.98</v>
-      </c>
-      <c r="H14">
-        <f>H10</f>
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>15</v>
-      </c>
-      <c r="D15">
-        <v>20</v>
-      </c>
-      <c r="E15">
-        <v>25</v>
-      </c>
-      <c r="F15">
-        <v>60</v>
-      </c>
-      <c r="G15">
-        <v>2.98</v>
-      </c>
-      <c r="H15">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>8</v>
-      </c>
-      <c r="E16">
-        <v>12</v>
-      </c>
-      <c r="F16">
-        <v>20</v>
-      </c>
-      <c r="G16">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="H16">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>5</v>
-      </c>
-      <c r="F17">
-        <v>10</v>
-      </c>
-      <c r="G17">
-        <v>1.37</v>
-      </c>
-      <c r="H17">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>4</v>
-      </c>
-      <c r="E18">
-        <v>5</v>
-      </c>
-      <c r="F18">
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <f>G17</f>
-        <v>1.37</v>
-      </c>
-      <c r="H18">
-        <f>H17</f>
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>10</v>
-      </c>
-      <c r="E19">
-        <v>15</v>
-      </c>
-      <c r="F19">
-        <v>30</v>
-      </c>
-      <c r="G19">
-        <f>G8</f>
-        <v>2.21</v>
-      </c>
-      <c r="H19">
-        <f>H8</f>
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>4</v>
-      </c>
-      <c r="E20">
-        <v>6</v>
-      </c>
-      <c r="F20">
-        <v>10</v>
-      </c>
-      <c r="G20">
-        <v>1.3</v>
-      </c>
-      <c r="H20">
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>5</v>
-      </c>
-      <c r="D21">
-        <v>8</v>
-      </c>
-      <c r="E21">
-        <v>12</v>
-      </c>
-      <c r="F21">
-        <v>20</v>
-      </c>
-      <c r="G21" s="9">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="H21" s="9">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22">
-        <v>14</v>
-      </c>
-      <c r="E22">
-        <v>18</v>
-      </c>
-      <c r="F22">
-        <v>30</v>
-      </c>
-      <c r="G22">
-        <v>2.61</v>
-      </c>
-      <c r="H22">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>8</v>
-      </c>
-      <c r="D23">
-        <v>12</v>
-      </c>
-      <c r="E23">
-        <v>16</v>
-      </c>
-      <c r="F23">
-        <v>30</v>
-      </c>
-      <c r="G23">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="H23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24">
-        <v>10</v>
-      </c>
-      <c r="D24">
-        <v>14</v>
-      </c>
-      <c r="E24">
-        <v>18</v>
-      </c>
-      <c r="F24">
-        <v>30</v>
-      </c>
-      <c r="G24">
-        <f>G22</f>
-        <v>2.61</v>
-      </c>
-      <c r="H24">
-        <f>H22</f>
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-      <c r="D25">
-        <v>14</v>
-      </c>
-      <c r="E25">
-        <v>18</v>
-      </c>
-      <c r="F25">
-        <v>30</v>
-      </c>
-      <c r="G25">
-        <f>G22</f>
-        <v>2.61</v>
-      </c>
-      <c r="H25">
-        <f>H22</f>
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="str">
-        <f>'Backlog &amp; dependencies'!A26</f>
-        <v>6. Interface to parking fine system</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26">
-        <v>14</v>
-      </c>
-      <c r="E26">
-        <v>18</v>
-      </c>
-      <c r="F26">
-        <v>30</v>
-      </c>
-      <c r="G26">
-        <f>G22</f>
-        <v>2.61</v>
-      </c>
-      <c r="H26">
-        <f>H22</f>
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D27">
-        <f>SUM(D2:D26)</f>
-        <v>251</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J20"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2418,10 +1736,10 @@
         <v>Work Items</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>47</v>
@@ -2618,7 +1936,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7">
         <v>30</v>
@@ -2651,7 +1969,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>20</v>
@@ -2684,7 +2002,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9">
         <v>20</v>
@@ -2717,7 +2035,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -2750,7 +2068,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11">
         <v>15</v>
@@ -2783,7 +2101,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12">
         <v>15</v>
@@ -2818,7 +2136,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13">
         <v>50</v>
@@ -2851,7 +2169,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14">
         <v>15</v>
@@ -2884,7 +2202,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15">
         <v>50</v>
@@ -2917,7 +2235,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -2950,7 +2268,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -2983,7 +2301,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18">
         <v>15</v>
@@ -3016,7 +2334,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19">
         <v>50</v>
@@ -3051,7 +2369,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -3095,14 +2413,14 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24">
         <v>250000</v>
@@ -3112,7 +2430,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B25">
         <v>97000</v>
@@ -3120,7 +2438,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26">
         <v>40000</v>
@@ -3128,7 +2446,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27">
         <v>2600</v>
@@ -3136,7 +2454,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28">
         <v>1200</v>
@@ -3147,12 +2465,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F25"/>
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3177,21 +2496,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>3.9710000000000001</v>
+        <v>1.7470000000000001</v>
       </c>
       <c r="C2">
-        <v>0.193</v>
-      </c>
-      <c r="D2">
-        <v>2.7360000000000002</v>
-      </c>
-      <c r="E2">
-        <v>0.47499999999999998</v>
+        <v>0.73</v>
+      </c>
+      <c r="D2" s="9">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="E2" s="9">
+        <v>1.04</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -3202,16 +2521,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>4.5659999999999998</v>
+        <v>2.61</v>
       </c>
       <c r="C3">
-        <v>0.14299999999999999</v>
+        <v>0.65</v>
       </c>
       <c r="D3">
-        <v>3.4380000000000002</v>
+        <v>2.97</v>
       </c>
       <c r="E3">
-        <v>0.48799999999999999</v>
+        <v>0.75</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -3222,16 +2541,18 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>3.492</v>
+        <v>1.88</v>
       </c>
       <c r="C4">
-        <v>0.32200000000000001</v>
+        <v>0.64</v>
       </c>
       <c r="D4">
-        <v>3.0950000000000002</v>
+        <f>D2</f>
+        <v>2.5099999999999998</v>
       </c>
       <c r="E4">
-        <v>0.42299999999999999</v>
+        <f>E2</f>
+        <v>1.04</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -3242,16 +2563,20 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>3.1760000000000002</v>
+        <f>B2</f>
+        <v>1.7470000000000001</v>
       </c>
       <c r="C5">
-        <v>0.29199999999999998</v>
+        <f>C2</f>
+        <v>0.73</v>
       </c>
       <c r="D5">
-        <v>3.379</v>
+        <f>D3</f>
+        <v>2.97</v>
       </c>
       <c r="E5">
-        <v>0.67200000000000004</v>
+        <f>E3</f>
+        <v>0.75</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -3262,16 +2587,18 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>4.0259999999999998</v>
+        <v>2.35</v>
       </c>
       <c r="C6">
-        <v>0.32200000000000001</v>
+        <v>0.65</v>
       </c>
       <c r="D6">
-        <v>3.528</v>
+        <f>D2</f>
+        <v>2.5099999999999998</v>
       </c>
       <c r="E6">
-        <v>0.40100000000000002</v>
+        <f>E2</f>
+        <v>1.04</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
@@ -3282,16 +2609,18 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>4.4530000000000003</v>
+        <f>B3</f>
+        <v>2.61</v>
       </c>
       <c r="C7">
-        <v>0.23699999999999999</v>
+        <f>C3</f>
+        <v>0.65</v>
       </c>
       <c r="D7">
-        <v>3.1720000000000002</v>
+        <v>3.42</v>
       </c>
       <c r="E7">
-        <v>0.58699999999999997</v>
+        <v>0.65</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -3302,16 +2631,19 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>3.5680000000000001</v>
+        <v>2.21</v>
       </c>
       <c r="C8">
-        <v>0.251</v>
+        <v>0.75</v>
       </c>
       <c r="D8">
-        <v>3.448</v>
+        <v>3.55</v>
       </c>
       <c r="E8">
-        <v>0.51200000000000001</v>
+        <v>0.67</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3319,19 +2651,19 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>3.823</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="C9">
-        <v>0.309</v>
+        <v>0.88</v>
       </c>
       <c r="D9">
-        <v>2.992</v>
+        <v>3.02</v>
       </c>
       <c r="E9">
-        <v>0.81799999999999995</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
+        <v>1.05</v>
+      </c>
+      <c r="F9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -3339,16 +2671,16 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>3.3319999999999999</v>
+        <v>1.98</v>
       </c>
       <c r="C10">
-        <v>0.156</v>
+        <v>0.71</v>
       </c>
       <c r="D10">
-        <v>3.3450000000000002</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="E10">
-        <v>0.51600000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="F10">
         <v>4</v>
@@ -3359,16 +2691,18 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>3.3319999999999999</v>
+        <f>B10</f>
+        <v>1.98</v>
       </c>
       <c r="C11">
-        <v>0.157</v>
+        <f>C10</f>
+        <v>0.71</v>
       </c>
       <c r="D11">
-        <v>3.7</v>
+        <v>2.09</v>
       </c>
       <c r="E11">
-        <v>0.52400000000000002</v>
+        <v>0.82</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
@@ -3379,16 +2713,20 @@
         <v>18</v>
       </c>
       <c r="B12">
-        <v>3.5510000000000002</v>
+        <f>B10</f>
+        <v>1.98</v>
       </c>
       <c r="C12">
-        <v>0.192</v>
+        <f>C10</f>
+        <v>0.71</v>
       </c>
       <c r="D12">
-        <v>3.919</v>
+        <f>D2</f>
+        <v>2.5099999999999998</v>
       </c>
       <c r="E12">
-        <v>0.41099999999999998</v>
+        <f>E2</f>
+        <v>1.04</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -3399,16 +2737,18 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>4.2409999999999997</v>
+        <f>B3</f>
+        <v>2.61</v>
       </c>
       <c r="C13">
-        <v>0.20200000000000001</v>
+        <f>C3</f>
+        <v>0.65</v>
       </c>
       <c r="D13">
-        <v>3.9860000000000002</v>
+        <v>3.13</v>
       </c>
       <c r="E13">
-        <v>0.64</v>
+        <v>1.03</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -3419,16 +2759,18 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>3.827</v>
+        <f>B10</f>
+        <v>1.98</v>
       </c>
       <c r="C14">
-        <v>0.317</v>
+        <f>C10</f>
+        <v>0.71</v>
       </c>
       <c r="D14">
-        <v>3.7429999999999999</v>
+        <v>2.73</v>
       </c>
       <c r="E14">
-        <v>0.505</v>
+        <v>0.65</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -3439,16 +2781,16 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>4.306</v>
+        <v>2.98</v>
       </c>
       <c r="C15">
-        <v>0.191</v>
+        <v>0.38</v>
       </c>
       <c r="D15">
-        <v>2.7440000000000002</v>
+        <v>3.09</v>
       </c>
       <c r="E15">
-        <v>0.59599999999999997</v>
+        <v>1.02</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -3459,16 +2801,16 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>3.5680000000000001</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="C16">
-        <v>0.251</v>
+        <v>0.59</v>
       </c>
       <c r="D16">
-        <v>3.4260000000000002</v>
+        <v>3.33</v>
       </c>
       <c r="E16">
-        <v>0.46899999999999997</v>
+        <v>0.71</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -3479,16 +2821,16 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>3.4980000000000002</v>
+        <v>1.37</v>
       </c>
       <c r="C17">
-        <v>0.29399999999999998</v>
+        <v>0.38</v>
       </c>
       <c r="D17">
-        <v>2.7</v>
+        <v>1.66</v>
       </c>
       <c r="E17">
-        <v>0.54800000000000004</v>
+        <v>0.9</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
@@ -3499,16 +2841,18 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <v>3.5219999999999998</v>
+        <f>B17</f>
+        <v>1.37</v>
       </c>
       <c r="C18">
-        <v>0.13300000000000001</v>
+        <f>C17</f>
+        <v>0.38</v>
       </c>
       <c r="D18">
-        <v>3.0630000000000002</v>
+        <v>3.42</v>
       </c>
       <c r="E18">
-        <v>0.46700000000000003</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -3516,16 +2860,23 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <v>4.0190000000000001</v>
+        <f>B8</f>
+        <v>2.21</v>
       </c>
       <c r="C19">
-        <v>0.16300000000000001</v>
+        <f>C8</f>
+        <v>0.75</v>
       </c>
       <c r="D19">
-        <v>2.581</v>
+        <f>D17</f>
+        <v>1.66</v>
       </c>
       <c r="E19">
-        <v>0.623</v>
+        <f>E17</f>
+        <v>0.9</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3533,27 +2884,27 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <v>3.306</v>
+        <v>1.3</v>
       </c>
       <c r="C20">
-        <v>0.17</v>
+        <v>0.69</v>
       </c>
       <c r="D20">
-        <v>2.2309999999999999</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="E20">
-        <v>0.77500000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21">
-        <v>3.819</v>
-      </c>
-      <c r="C21">
-        <v>0.19800000000000001</v>
+      <c r="B21" s="9">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0.59</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -3567,10 +2918,10 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>3.5510000000000002</v>
+        <v>2.61</v>
       </c>
       <c r="C22">
-        <v>0.192</v>
+        <v>0.42</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -3584,10 +2935,10 @@
         <v>3</v>
       </c>
       <c r="B23">
-        <v>4.2839999999999998</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="C23">
-        <v>0.25800000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -3601,10 +2952,12 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>3.415</v>
+        <f>B22</f>
+        <v>2.61</v>
       </c>
       <c r="C24">
-        <v>0.21299999999999999</v>
+        <f>C22</f>
+        <v>0.42</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -3618,15 +2971,36 @@
         <v>5</v>
       </c>
       <c r="B25">
-        <v>3.8530000000000002</v>
+        <f>B22</f>
+        <v>2.61</v>
       </c>
       <c r="C25">
-        <v>0.16400000000000001</v>
+        <f>C22</f>
+        <v>0.42</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <f>B22</f>
+        <v>2.61</v>
+      </c>
+      <c r="C26">
+        <f>C22</f>
+        <v>0.42</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
         <v>0</v>
       </c>
     </row>

</xml_diff>